<commit_message>
Translate everything in English
</commit_message>
<xml_diff>
--- a/power-plant-informations.xlsx
+++ b/power-plant-informations.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rs3753e\sciebo\Vorlesungen\WiSe_MnM Flex\Teil II\VL 1 Intrinsic Rolling\IR Optimierung MILP Tagesbetrachtung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Workspace\hydro-power-trading\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B03EB7-AA9E-4184-9D56-DDFA6F45653B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8D5B88-E53A-43BD-A4C4-7F5D8EBEB009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="17250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="ps1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,43 +27,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
-    <t>Turbinierwirkungsgrad</t>
-  </si>
-  <si>
-    <t>Pumpwirkungsgrad</t>
-  </si>
-  <si>
-    <t>MWh/h</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
     <t>MWh</t>
   </si>
   <si>
-    <t>Einheit</t>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
-    <t>Turbinierleistung Netto max</t>
-  </si>
-  <si>
-    <t>Turbinierleistung Netto min</t>
-  </si>
-  <si>
-    <t>Speicher 1</t>
-  </si>
-  <si>
-    <t>Arbeitsvolumen Netto</t>
-  </si>
-  <si>
-    <t>Pumpleistung Brutto max</t>
-  </si>
-  <si>
-    <t>Pumpleistung Brutto min</t>
+    <t>Turbine power (net) max</t>
+  </si>
+  <si>
+    <t>Turbine power (net)min</t>
+  </si>
+  <si>
+    <t>Pump power (gross) max</t>
+  </si>
+  <si>
+    <t>Pumpleistung (gross) min</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>Turbine efficiency</t>
+  </si>
+  <si>
+    <t>Pump efficiency</t>
+  </si>
+  <si>
+    <t>Net energy capacity</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Pump storage 1</t>
   </si>
 </sst>
 </file>
@@ -400,97 +400,97 @@
   <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
       </c>
       <c r="C3" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C8" s="3">
         <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2">
         <v>600</v>

</xml_diff>